<commit_message>
added restsharp and an api test
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="user stories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>FULL STACK DEVELOPER TESZT FELADAT</t>
   </si>
@@ -164,6 +165,78 @@
   </si>
   <si>
     <t>not part of the scope, but worth considering..</t>
+  </si>
+  <si>
+    <t>web authorization is not in scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>not needed</t>
+  </si>
+  <si>
+    <t>git created</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>name 120 characters long</t>
+  </si>
+  <si>
+    <t>check length</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>EF 6.0</t>
+  </si>
+  <si>
+    <t>what if service is down?</t>
+  </si>
+  <si>
+    <t>validate on textchanged</t>
+  </si>
+  <si>
+    <t>quick feedback</t>
+  </si>
+  <si>
+    <t>validate at server before create</t>
+  </si>
+  <si>
+    <t>ensuring integrity</t>
+  </si>
+  <si>
+    <t>autofill for email?</t>
+  </si>
+  <si>
+    <t>improves comfort, reduces security?</t>
+  </si>
+  <si>
+    <t>I need to identify myself properly</t>
+  </si>
+  <si>
+    <t>As an administrator of products..</t>
+  </si>
+  <si>
+    <t>valid e-mail</t>
+  </si>
+  <si>
+    <t>All data is visible on one screen without scrolling</t>
+  </si>
+  <si>
+    <t>I'm well informed about the state of the action I'm doing</t>
+  </si>
+  <si>
+    <t>I can filter a list of products</t>
+  </si>
+  <si>
+    <t>I can easily select a category for a product</t>
+  </si>
+  <si>
+    <t>I need notifications when something is missing</t>
   </si>
 </sst>
 </file>
@@ -208,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -216,12 +289,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF4B4B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF4B4B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF4B4B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF4B4B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF4B4B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF4B4B"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFD5151"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -496,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,17 +696,33 @@
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -535,8 +738,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -546,8 +752,14 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+1</f>
         <v>2</v>
@@ -558,10 +770,13 @@
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" ref="A8:A39" si="0">A7+1</f>
+        <f t="shared" ref="A8:A60" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" t="s">
@@ -571,7 +786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -583,7 +798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -595,7 +810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -607,7 +822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -618,8 +833,11 @@
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -631,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A13+1</f>
         <v>9</v>
@@ -642,26 +860,32 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>13</v>
@@ -673,7 +897,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>13</v>
@@ -685,7 +909,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>13</v>
@@ -700,7 +924,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>13</v>
@@ -712,7 +936,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>13</v>
@@ -724,7 +948,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>13</v>
@@ -739,7 +963,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>13</v>
@@ -750,35 +974,38 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -787,7 +1014,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>13</v>
@@ -799,7 +1026,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>13</v>
@@ -808,25 +1035,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>13</v>
@@ -838,7 +1065,7 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>13</v>
@@ -850,7 +1077,7 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>13</v>
@@ -862,7 +1089,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>13</v>
@@ -874,7 +1101,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>13</v>
@@ -886,7 +1113,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>13</v>
@@ -898,7 +1125,7 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>13</v>
@@ -906,14 +1133,17 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f>A35+1</f>
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,17 +1151,266 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="3">
+        <v>43417</v>
+      </c>
+      <c r="E38" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3">
+        <v>43417</v>
+      </c>
+      <c r="E39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="3">
+        <v>43417</v>
+      </c>
+      <c r="E40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B16:B36">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>AND(ISBLANK($D15),NOT(ISBLANK($C15)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="11">
+      <formula>AND(NOT(ISBLANK($D15)),NOT(ISBLANK($C15)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="12">
+      <formula>ISBLANK($D15)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:XFD1048576 A36:A1048576">
+    <cfRule type="expression" dxfId="5" priority="16" stopIfTrue="1">
+      <formula>AND(ISBLANK($D37),NOT(ISBLANK($C37)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="17">
+      <formula>AND(NOT(ISBLANK($D37)),NOT(ISBLANK($C37)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="18">
+      <formula>ISBLANK($D37)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>AND(ISBLANK($D1),NOT(ISBLANK($C1)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(NOT(ISBLANK($D1)),NOT(ISBLANK($C1)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>ISBLANK($D1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>